<commit_message>
No way stekelbaars of 409 and 468 grams
</commit_message>
<xml_diff>
--- a/data/biotiek/vis/elektrisch/extern/verwerkt_in_excel/vis_elektrisch.xlsx
+++ b/data/biotiek/vis/elektrisch/extern/verwerkt_in_excel/vis_elektrisch.xlsx
@@ -415,8 +415,8 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G117" sqref="G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3802,7 +3802,7 @@
         <v>75</v>
       </c>
       <c r="H124" s="7">
-        <v>409</v>
+        <v>4.09</v>
       </c>
       <c r="I124" s="8"/>
     </row>
@@ -3829,7 +3829,7 @@
         <v>53</v>
       </c>
       <c r="H125" s="7">
-        <v>468</v>
+        <v>4.68</v>
       </c>
       <c r="I125" s="8"/>
     </row>

</xml_diff>